<commit_message>
anh truc + techglobal
</commit_message>
<xml_diff>
--- a/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang12/2.XulyBH/XLBH2212_Duphonglapdat.xlsx
+++ b/5. WS/1. Bộ phận bảo hành/1. Thực hiện sửa chữa bảo hành/nam2022/Thang12/2.XulyBH/XLBH2212_Duphonglapdat.xlsx
@@ -22,14 +22,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TG102'!$S$4:$S$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TG102LE!$S$4:$S$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">TG102LE!$S$4:$S$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'TG102LE-4G'!$S$4:$S$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">TG102SE!$S$4:$S$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">TG102V!$S$4:$S$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">TongThang!$S$4:$S$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TOP-1'!$S$4:$S$51</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="0">'TG102'!$S$4:$S$51</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="3">TG102LE!$S$4:$S$51</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="3">TG102LE!$S$4:$S$53</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="2">'TG102LE-4G'!$S$4:$S$51</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="4">TG102SE!$S$4:$S$51</definedName>
     <definedName name="_xlnm.Criteria" localSheetId="5">TG102V!$S$4:$S$51</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="146">
   <si>
     <t>STT</t>
   </si>
@@ -460,6 +460,30 @@
   </si>
   <si>
     <t>Thế module GSM/GPS qua Imei: 868183037834327</t>
+  </si>
+  <si>
+    <t>Main chập nổ thiếu nhiều LK</t>
+  </si>
+  <si>
+    <t>NG,LK</t>
+  </si>
+  <si>
+    <t>Thiết bị lỗi module GSM</t>
+  </si>
+  <si>
+    <t>Thiết bị chập MCU linh, tụ trở hàn sai, mất ID</t>
+  </si>
+  <si>
+    <t>Thay MCU, xử lý lại main, nạp lại FW module GSM</t>
+  </si>
+  <si>
+    <t>MCU,NCFW,LK</t>
+  </si>
+  <si>
+    <t>Sai Imei</t>
+  </si>
+  <si>
+    <t>Khởi tạo lại thiết bị</t>
   </si>
 </sst>
 </file>
@@ -910,30 +934,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -951,6 +951,30 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1294,41 +1318,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="95"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -1373,58 +1397,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="80" t="s">
         <v>1</v>
       </c>
@@ -1449,23 +1473,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="80" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1497,7 +1521,7 @@
       <c r="R6" s="64"/>
       <c r="S6" s="3"/>
       <c r="T6" s="81"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -1534,7 +1558,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="81"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -1569,7 +1593,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="81"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1604,7 +1628,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="81"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -1639,7 +1663,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="81"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -1674,7 +1698,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="81"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -1709,7 +1733,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="81"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -1746,7 +1770,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="81"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -1781,7 +1805,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="81"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1816,7 +1840,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1845,7 +1869,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3561,6 +3585,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -3572,13 +3603,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3622,39 +3646,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -3699,58 +3723,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
@@ -3775,23 +3799,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="65" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -3823,7 +3847,7 @@
       <c r="R6" s="64"/>
       <c r="S6" s="3"/>
       <c r="T6" s="66"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -3860,7 +3884,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="66"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -3895,7 +3919,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -3924,7 +3948,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -3953,7 +3977,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="66"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -3982,7 +4006,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="66"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -4011,7 +4035,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="66"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -4042,7 +4066,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="66"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -4071,7 +4095,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -4100,7 +4124,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4129,7 +4153,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5845,13 +5869,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -5863,6 +5880,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5906,39 +5930,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -5983,58 +6007,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
@@ -6059,23 +6083,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="65" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6107,7 +6131,7 @@
       <c r="R6" s="64"/>
       <c r="S6" s="3"/>
       <c r="T6" s="66"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -6144,7 +6168,7 @@
       <c r="R7" s="64"/>
       <c r="S7" s="3"/>
       <c r="T7" s="66"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -6179,7 +6203,7 @@
       <c r="R8" s="64"/>
       <c r="S8" s="3"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -6214,7 +6238,7 @@
       <c r="R9" s="64"/>
       <c r="S9" s="3"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -6249,7 +6273,7 @@
       <c r="R10" s="64"/>
       <c r="S10" s="3"/>
       <c r="T10" s="66"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -6284,7 +6308,7 @@
       <c r="R11" s="64"/>
       <c r="S11" s="3"/>
       <c r="T11" s="66"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -6319,7 +6343,7 @@
       <c r="R12" s="64"/>
       <c r="S12" s="3"/>
       <c r="T12" s="66"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -6350,7 +6374,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="66"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -6379,7 +6403,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -6408,7 +6432,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -6437,7 +6461,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -8153,13 +8177,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -8171,6 +8188,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8179,10 +8203,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X115"/>
+  <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8214,41 +8238,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="95"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -8293,58 +8317,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
@@ -8369,23 +8393,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="65" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -8435,7 +8459,7 @@
       </c>
       <c r="S6" s="68"/>
       <c r="T6" s="66"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -8490,7 +8514,7 @@
       </c>
       <c r="S7" s="68"/>
       <c r="T7" s="66"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -8547,7 +8571,7 @@
       </c>
       <c r="S8" s="68"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -8602,7 +8626,7 @@
       </c>
       <c r="S9" s="68"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -8659,7 +8683,7 @@
       </c>
       <c r="S10" s="68"/>
       <c r="T10" s="66"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -8710,7 +8734,7 @@
       </c>
       <c r="S11" s="68"/>
       <c r="T11" s="66"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -8747,7 +8771,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="66"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -8800,7 +8824,7 @@
       </c>
       <c r="S13" s="3"/>
       <c r="T13" s="66"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -8835,7 +8859,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -8886,7 +8910,7 @@
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -8937,7 +8961,7 @@
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -9111,24 +9135,40 @@
       <c r="F20" s="47"/>
       <c r="G20" s="37"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="I20" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
+      <c r="M20" s="39" t="s">
+        <v>145</v>
+      </c>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="2"/>
+      <c r="O20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P20" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="S20" s="3"/>
       <c r="T20" s="13"/>
       <c r="U20" s="9" t="s">
         <v>17</v>
       </c>
       <c r="V20" s="9">
-        <f>COUNTIF($Q$6:$Q$51,"PM")</f>
-        <v>7</v>
+        <f>COUNTIF($Q$6:$Q$53,"PM")</f>
+        <v>8</v>
       </c>
       <c r="W20" s="13"/>
     </row>
@@ -9149,24 +9189,40 @@
       <c r="F21" s="47"/>
       <c r="G21" s="37"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="51"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="I21" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
+      <c r="M21" s="39" t="s">
+        <v>124</v>
+      </c>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="2"/>
+      <c r="O21" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P21" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="S21" s="3"/>
       <c r="T21" s="13"/>
       <c r="U21" s="9" t="s">
         <v>49</v>
       </c>
       <c r="V21" s="9">
-        <f>COUNTIF($Q$6:$Q$51,"PC")</f>
-        <v>9</v>
+        <f>COUNTIF($Q$6:$Q$53,"PC")</f>
+        <v>11</v>
       </c>
       <c r="W21" s="13"/>
     </row>
@@ -9203,8 +9259,8 @@
         <v>50</v>
       </c>
       <c r="V22" s="9">
-        <f>COUNTIF($Q$6:$Q$51,"PC+PM")</f>
-        <v>2</v>
+        <f>COUNTIF($Q$6:$Q$53,"PC+PM")</f>
+        <v>3</v>
       </c>
       <c r="W22" s="13"/>
     </row>
@@ -9360,8 +9416,8 @@
         <v>26</v>
       </c>
       <c r="V26" s="9">
-        <f>COUNTIF($R$6:$R$51,"*MCU*")</f>
-        <v>2</v>
+        <f>COUNTIF($R$6:$R$53,"*MCU*")</f>
+        <v>3</v>
       </c>
       <c r="W26" s="13"/>
     </row>
@@ -9416,8 +9472,8 @@
         <v>34</v>
       </c>
       <c r="V27" s="9">
-        <f>COUNTIF($R$6:$R$51,"*GSM*")</f>
-        <v>3</v>
+        <f>COUNTIF($R$6:$R$53,"*GSM*")</f>
+        <v>4</v>
       </c>
       <c r="W27" s="13"/>
     </row>
@@ -9472,7 +9528,7 @@
         <v>27</v>
       </c>
       <c r="V28" s="9">
-        <f>COUNTIF($R$6:$R$51,"*GPS*")</f>
+        <f>COUNTIF($R$6:$R$53,"*GPS*")</f>
         <v>1</v>
       </c>
       <c r="W28" s="13"/>
@@ -9526,8 +9582,8 @@
         <v>52</v>
       </c>
       <c r="V29" s="9">
-        <f>COUNTIF($R$6:$R$51,"*NG*")</f>
-        <v>3</v>
+        <f>COUNTIF($R$6:$R$53,"*NG*")</f>
+        <v>4</v>
       </c>
       <c r="W29" s="13"/>
     </row>
@@ -9564,7 +9620,7 @@
         <v>32</v>
       </c>
       <c r="V30" s="9">
-        <f>COUNTIF($R$6:$R$51,"*I/O*")</f>
+        <f>COUNTIF($R$6:$R$53,"*I/O*")</f>
         <v>0</v>
       </c>
       <c r="W30" s="13"/>
@@ -9616,8 +9672,8 @@
         <v>22</v>
       </c>
       <c r="V31" s="9">
-        <f>COUNTIF($R$6:$R$51,"*LK*")</f>
-        <v>5</v>
+        <f>COUNTIF($R$6:$R$53,"*LK*")</f>
+        <v>7</v>
       </c>
       <c r="W31" s="13"/>
     </row>
@@ -9658,7 +9714,7 @@
         <v>28</v>
       </c>
       <c r="V32" s="9">
-        <f>COUNTIF($R$6:$R$51,"*MCH*")</f>
+        <f>COUNTIF($R$6:$R$53,"*MCH*")</f>
         <v>0</v>
       </c>
       <c r="W32" s="13"/>
@@ -9696,8 +9752,8 @@
         <v>47</v>
       </c>
       <c r="V33" s="9">
-        <f>COUNTIF($R$6:$R$51,"*SF*")</f>
-        <v>1</v>
+        <f>COUNTIF($R$6:$R$53,"*SF*")</f>
+        <v>2</v>
       </c>
       <c r="W33" s="13"/>
     </row>
@@ -9719,22 +9775,34 @@
       <c r="G34" s="37"/>
       <c r="H34" s="1"/>
       <c r="I34" s="51"/>
-      <c r="J34" s="1"/>
+      <c r="J34" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="K34" s="1"/>
       <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
+      <c r="M34" s="39" t="s">
+        <v>124</v>
+      </c>
       <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="2"/>
+      <c r="O34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P34" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>139</v>
+      </c>
       <c r="S34" s="3"/>
       <c r="T34" s="13"/>
       <c r="U34" s="3" t="s">
         <v>48</v>
       </c>
       <c r="V34" s="9">
-        <f>COUNTIF($R$6:$R$51,"*RTB*")</f>
+        <f>COUNTIF($R$6:$R$53,"*RTB*")</f>
         <v>0</v>
       </c>
       <c r="W34" s="13"/>
@@ -9788,8 +9856,8 @@
         <v>38</v>
       </c>
       <c r="V35" s="9">
-        <f>COUNTIF($R$6:$R$51,"*NCFW*")</f>
-        <v>2</v>
+        <f>COUNTIF($R$6:$R$53,"*NCFW*")</f>
+        <v>3</v>
       </c>
       <c r="W35" s="13"/>
     </row>
@@ -9828,15 +9896,13 @@
         <v>29</v>
       </c>
       <c r="V36" s="9">
-        <f>COUNTIF($R$6:$R$51,"*KL*")</f>
+        <f>COUNTIF($R$6:$R$53,"*KL*")</f>
         <v>5</v>
       </c>
       <c r="W36" s="13"/>
     </row>
     <row r="37" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>32</v>
-      </c>
+      <c r="A37" s="3"/>
       <c r="B37" s="58">
         <v>44921</v>
       </c>
@@ -9844,17 +9910,17 @@
       <c r="D37" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="E37" s="67" t="s">
-        <v>106</v>
+      <c r="E37" s="67">
+        <v>868183034585575</v>
       </c>
       <c r="F37" s="47"/>
       <c r="G37" s="37"/>
-      <c r="H37" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="H37" s="1"/>
       <c r="I37" s="51"/>
       <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="K37" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="L37" s="39"/>
       <c r="M37" s="39"/>
       <c r="N37" s="1"/>
@@ -9864,53 +9930,76 @@
       <c r="R37" s="2"/>
       <c r="S37" s="3"/>
       <c r="T37" s="13"/>
-      <c r="U37" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="V37" s="9">
-        <f>SUM(V26:V36)</f>
-        <v>22</v>
-      </c>
+      <c r="U37" s="3"/>
+      <c r="V37" s="9"/>
       <c r="W37" s="13"/>
     </row>
     <row r="38" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>33</v>
-      </c>
-      <c r="B38" s="54"/>
+      <c r="A38" s="3"/>
+      <c r="B38" s="58">
+        <v>44921</v>
+      </c>
       <c r="C38" s="54"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
+      <c r="D38" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="67">
+        <v>868183038478751</v>
+      </c>
       <c r="F38" s="47"/>
       <c r="G38" s="37"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="1"/>
+      <c r="I38" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="K38" s="1"/>
-      <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
+      <c r="L38" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="M38" s="39" t="s">
+        <v>142</v>
+      </c>
       <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="2"/>
+      <c r="O38" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P38" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="R38" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="S38" s="3"/>
       <c r="T38" s="13"/>
-      <c r="U38" s="13"/>
-      <c r="V38" s="15"/>
+      <c r="U38" s="3"/>
+      <c r="V38" s="9"/>
       <c r="W38" s="13"/>
     </row>
     <row r="39" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>34</v>
-      </c>
-      <c r="B39" s="54"/>
+        <v>32</v>
+      </c>
+      <c r="B39" s="58">
+        <v>44921</v>
+      </c>
       <c r="C39" s="54"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38"/>
+      <c r="D39" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>106</v>
+      </c>
       <c r="F39" s="47"/>
       <c r="G39" s="37"/>
-      <c r="H39" s="1"/>
+      <c r="H39" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="I39" s="51"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -9923,13 +10012,18 @@
       <c r="R39" s="2"/>
       <c r="S39" s="3"/>
       <c r="T39" s="13"/>
-      <c r="U39" s="13"/>
-      <c r="V39" s="15"/>
+      <c r="U39" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="V39" s="9">
+        <f>SUM(V26:V36)</f>
+        <v>29</v>
+      </c>
       <c r="W39" s="13"/>
     </row>
     <row r="40" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B40" s="54"/>
       <c r="C40" s="54"/>
@@ -9950,18 +10044,13 @@
       <c r="R40" s="2"/>
       <c r="S40" s="3"/>
       <c r="T40" s="13"/>
-      <c r="U40" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="V40" s="9">
-        <f>COUNTIF($O$6:$O$51,"*DM*")</f>
-        <v>0</v>
-      </c>
+      <c r="U40" s="13"/>
+      <c r="V40" s="15"/>
       <c r="W40" s="13"/>
     </row>
     <row r="41" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B41" s="54"/>
       <c r="C41" s="54"/>
@@ -9982,18 +10071,13 @@
       <c r="R41" s="2"/>
       <c r="S41" s="3"/>
       <c r="T41" s="13"/>
-      <c r="U41" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="V41" s="9">
-        <f>COUNTIF($O$6:$O$51,"*KS*")</f>
-        <v>1</v>
-      </c>
+      <c r="U41" s="13"/>
+      <c r="V41" s="15"/>
       <c r="W41" s="13"/>
     </row>
     <row r="42" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" s="54"/>
       <c r="C42" s="54"/>
@@ -10014,13 +10098,18 @@
       <c r="R42" s="2"/>
       <c r="S42" s="3"/>
       <c r="T42" s="13"/>
-      <c r="U42" s="13"/>
-      <c r="V42" s="15"/>
+      <c r="U42" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="V42" s="9">
+        <f>COUNTIF($O$6:$O$53,"*DM*")</f>
+        <v>0</v>
+      </c>
       <c r="W42" s="13"/>
     </row>
     <row r="43" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B43" s="54"/>
       <c r="C43" s="54"/>
@@ -10041,13 +10130,18 @@
       <c r="R43" s="2"/>
       <c r="S43" s="3"/>
       <c r="T43" s="13"/>
-      <c r="U43" s="13"/>
-      <c r="V43" s="15"/>
+      <c r="U43" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="V43" s="9">
+        <f>COUNTIF($O$6:$O$53,"*KS*")</f>
+        <v>3</v>
+      </c>
       <c r="W43" s="13"/>
     </row>
     <row r="44" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" s="54"/>
       <c r="C44" s="54"/>
@@ -10068,22 +10162,13 @@
       <c r="R44" s="2"/>
       <c r="S44" s="3"/>
       <c r="T44" s="13"/>
-      <c r="U44" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="V44" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="W44" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="X44" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="U44" s="13"/>
+      <c r="V44" s="15"/>
+      <c r="W44" s="13"/>
     </row>
     <row r="45" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B45" s="54"/>
       <c r="C45" s="54"/>
@@ -10104,25 +10189,13 @@
       <c r="R45" s="2"/>
       <c r="S45" s="3"/>
       <c r="T45" s="13"/>
-      <c r="U45" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="V45" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE",$H$6:$H$300,"*Lô 3-20*")</f>
-        <v>0</v>
-      </c>
-      <c r="W45" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE",$H$6:$H$300,"*Lô 1-21*")</f>
-        <v>0</v>
-      </c>
-      <c r="X45" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE",$H$6:$H$300,"*Lô 2-21*")</f>
-        <v>0</v>
-      </c>
+      <c r="U45" s="13"/>
+      <c r="V45" s="15"/>
+      <c r="W45" s="13"/>
     </row>
     <row r="46" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B46" s="54"/>
       <c r="C46" s="54"/>
@@ -10144,24 +10217,21 @@
       <c r="S46" s="3"/>
       <c r="T46" s="13"/>
       <c r="U46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="V46" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE-4G",$H$6:$H$300,"*Lô 3-20*")</f>
-        <v>0</v>
-      </c>
-      <c r="W46" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE-4G",$H$6:$H$300,"*Lô 1-21*")</f>
-        <v>0</v>
-      </c>
-      <c r="X46" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102LE-4G",$H$6:$H$300,"*Lô 2-21*")</f>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="V46" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="W46" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="X46" s="9" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B47" s="54"/>
       <c r="C47" s="54"/>
@@ -10183,24 +10253,24 @@
       <c r="S47" s="3"/>
       <c r="T47" s="13"/>
       <c r="U47" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V47" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102E",$H$6:$H$300,"*Lô 3-20*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE",$H$6:$H$302,"*Lô 3-20*")</f>
         <v>0</v>
       </c>
       <c r="W47" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102E",$H$6:$H$300,"*Lô 1-21*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE",$H$6:$H$302,"*Lô 1-21*")</f>
         <v>0</v>
       </c>
       <c r="X47" s="9">
-        <f>COUNTIFS($D$6:$D$300,"TG102E",$H$6:$H$300,"*Lô 2-21*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE",$H$6:$H$302,"*Lô 2-21*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B48" s="54"/>
       <c r="C48" s="54"/>
@@ -10220,29 +10290,26 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="2"/>
       <c r="S48" s="3"/>
-      <c r="T48" s="34">
-        <f>COUNTIF(J9:J20,"*GSM*")</f>
-        <v>3</v>
-      </c>
+      <c r="T48" s="13"/>
       <c r="U48" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="V48" s="9">
-        <f>COUNTIFS($D$6:$D$300,"ACT-01",$H$6:$H$300,"*Lô 3-20*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE-4G",$H$6:$H$302,"*Lô 3-20*")</f>
         <v>0</v>
       </c>
       <c r="W48" s="9">
-        <f>COUNTIFS($D$6:$D$300,"ACT-01",$H$6:$H$300,"*Lô 1-21*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE-4G",$H$6:$H$302,"*Lô 1-21*")</f>
         <v>0</v>
       </c>
       <c r="X48" s="9">
-        <f>COUNTIFS($D$6:$D$300,"ACT-01",$H$6:$H$300,"*Lô 2-21*")</f>
+        <f>COUNTIFS($D$6:$D$302,"TG102LE-4G",$H$6:$H$302,"*Lô 2-21*")</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B49" s="54"/>
       <c r="C49" s="54"/>
@@ -10262,15 +10329,26 @@
       <c r="Q49" s="1"/>
       <c r="R49" s="2"/>
       <c r="S49" s="3"/>
-      <c r="T49" s="34"/>
-      <c r="U49" s="43"/>
-      <c r="V49" s="43"/>
-      <c r="W49" s="43"/>
-      <c r="X49" s="32"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="V49" s="9">
+        <f>COUNTIFS($D$6:$D$302,"TG102E",$H$6:$H$302,"*Lô 3-20*")</f>
+        <v>0</v>
+      </c>
+      <c r="W49" s="9">
+        <f>COUNTIFS($D$6:$D$302,"TG102E",$H$6:$H$302,"*Lô 1-21*")</f>
+        <v>0</v>
+      </c>
+      <c r="X49" s="9">
+        <f>COUNTIFS($D$6:$D$302,"TG102E",$H$6:$H$302,"*Lô 2-21*")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28">
-        <v>45</v>
+      <c r="A50" s="3">
+        <v>43</v>
       </c>
       <c r="B50" s="54"/>
       <c r="C50" s="54"/>
@@ -10278,10 +10356,10 @@
       <c r="E50" s="38"/>
       <c r="F50" s="47"/>
       <c r="G50" s="37"/>
-      <c r="H50" s="31"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="51"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
       <c r="L50" s="39"/>
       <c r="M50" s="39"/>
       <c r="N50" s="1"/>
@@ -10289,16 +10367,30 @@
       <c r="P50" s="39"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="2"/>
-      <c r="S50" s="28"/>
-      <c r="T50" s="34"/>
-      <c r="U50" s="43"/>
-      <c r="V50" s="43"/>
-      <c r="W50" s="43"/>
-      <c r="X50" s="32"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="34">
+        <f>COUNTIF(J9:J20,"*GSM*")</f>
+        <v>3</v>
+      </c>
+      <c r="U50" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="V50" s="9">
+        <f>COUNTIFS($D$6:$D$302,"ACT-01",$H$6:$H$302,"*Lô 3-20*")</f>
+        <v>0</v>
+      </c>
+      <c r="W50" s="9">
+        <f>COUNTIFS($D$6:$D$302,"ACT-01",$H$6:$H$302,"*Lô 1-21*")</f>
+        <v>0</v>
+      </c>
+      <c r="X50" s="9">
+        <f>COUNTIFS($D$6:$D$302,"ACT-01",$H$6:$H$302,"*Lô 2-21*")</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B51" s="54"/>
       <c r="C51" s="54"/>
@@ -10317,7 +10409,7 @@
       <c r="P51" s="39"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="9"/>
+      <c r="S51" s="3"/>
       <c r="T51" s="34"/>
       <c r="U51" s="43"/>
       <c r="V51" s="43"/>
@@ -10325,8 +10417,8 @@
       <c r="X51" s="32"/>
     </row>
     <row r="52" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>47</v>
+      <c r="A52" s="28">
+        <v>45</v>
       </c>
       <c r="B52" s="54"/>
       <c r="C52" s="54"/>
@@ -10334,10 +10426,10 @@
       <c r="E52" s="38"/>
       <c r="F52" s="47"/>
       <c r="G52" s="37"/>
-      <c r="H52" s="32"/>
+      <c r="H52" s="31"/>
       <c r="I52" s="51"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
+      <c r="J52" s="31"/>
+      <c r="K52" s="31"/>
       <c r="L52" s="39"/>
       <c r="M52" s="39"/>
       <c r="N52" s="1"/>
@@ -10345,7 +10437,7 @@
       <c r="P52" s="39"/>
       <c r="Q52" s="1"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="32"/>
+      <c r="S52" s="28"/>
       <c r="T52" s="34"/>
       <c r="U52" s="43"/>
       <c r="V52" s="43"/>
@@ -10354,7 +10446,7 @@
     </row>
     <row r="53" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B53" s="54"/>
       <c r="C53" s="54"/>
@@ -10362,10 +10454,10 @@
       <c r="E53" s="38"/>
       <c r="F53" s="47"/>
       <c r="G53" s="37"/>
-      <c r="H53" s="32"/>
+      <c r="H53" s="1"/>
       <c r="I53" s="51"/>
-      <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
       <c r="L53" s="39"/>
       <c r="M53" s="39"/>
       <c r="N53" s="1"/>
@@ -10373,7 +10465,7 @@
       <c r="P53" s="39"/>
       <c r="Q53" s="1"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="32"/>
+      <c r="S53" s="9"/>
       <c r="T53" s="34"/>
       <c r="U53" s="43"/>
       <c r="V53" s="43"/>
@@ -10382,7 +10474,7 @@
     </row>
     <row r="54" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B54" s="54"/>
       <c r="C54" s="54"/>
@@ -10410,7 +10502,7 @@
     </row>
     <row r="55" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B55" s="54"/>
       <c r="C55" s="54"/>
@@ -10430,7 +10522,7 @@
       <c r="Q55" s="1"/>
       <c r="R55" s="2"/>
       <c r="S55" s="32"/>
-      <c r="T55" s="35"/>
+      <c r="T55" s="34"/>
       <c r="U55" s="43"/>
       <c r="V55" s="43"/>
       <c r="W55" s="43"/>
@@ -10438,7 +10530,7 @@
     </row>
     <row r="56" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" s="54"/>
       <c r="C56" s="54"/>
@@ -10458,13 +10550,15 @@
       <c r="Q56" s="1"/>
       <c r="R56" s="2"/>
       <c r="S56" s="32"/>
-      <c r="U56" s="24"/>
-      <c r="V56" s="24"/>
-      <c r="W56" s="24"/>
+      <c r="T56" s="34"/>
+      <c r="U56" s="43"/>
+      <c r="V56" s="43"/>
+      <c r="W56" s="43"/>
+      <c r="X56" s="32"/>
     </row>
     <row r="57" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B57" s="54"/>
       <c r="C57" s="54"/>
@@ -10484,13 +10578,15 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="2"/>
       <c r="S57" s="32"/>
-      <c r="U57" s="24"/>
-      <c r="V57" s="24"/>
-      <c r="W57" s="24"/>
+      <c r="T57" s="35"/>
+      <c r="U57" s="43"/>
+      <c r="V57" s="43"/>
+      <c r="W57" s="43"/>
+      <c r="X57" s="32"/>
     </row>
     <row r="58" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B58" s="54"/>
       <c r="C58" s="54"/>
@@ -10510,16 +10606,19 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="2"/>
       <c r="S58" s="32"/>
+      <c r="U58" s="24"/>
+      <c r="V58" s="24"/>
+      <c r="W58" s="24"/>
     </row>
     <row r="59" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B59" s="54"/>
       <c r="C59" s="54"/>
       <c r="D59" s="37"/>
       <c r="E59" s="38"/>
-      <c r="F59" s="37"/>
+      <c r="F59" s="47"/>
       <c r="G59" s="37"/>
       <c r="H59" s="32"/>
       <c r="I59" s="51"/>
@@ -10533,16 +10632,19 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="2"/>
       <c r="S59" s="32"/>
+      <c r="U59" s="24"/>
+      <c r="V59" s="24"/>
+      <c r="W59" s="24"/>
     </row>
     <row r="60" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B60" s="54"/>
       <c r="C60" s="54"/>
       <c r="D60" s="37"/>
       <c r="E60" s="38"/>
-      <c r="F60" s="37"/>
+      <c r="F60" s="47"/>
       <c r="G60" s="37"/>
       <c r="H60" s="32"/>
       <c r="I60" s="51"/>
@@ -10559,53 +10661,53 @@
     </row>
     <row r="61" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B61" s="54"/>
-      <c r="C61" s="32"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
       <c r="H61" s="32"/>
-      <c r="I61" s="52"/>
+      <c r="I61" s="51"/>
       <c r="J61" s="32"/>
       <c r="K61" s="32"/>
       <c r="L61" s="39"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
-      <c r="O61" s="32"/>
-      <c r="P61" s="32"/>
-      <c r="Q61" s="32"/>
-      <c r="R61" s="32"/>
+      <c r="M61" s="39"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="39"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="2"/>
       <c r="S61" s="32"/>
     </row>
     <row r="62" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B62" s="54"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
+      <c r="C62" s="54"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="38"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
       <c r="H62" s="32"/>
-      <c r="I62" s="52"/>
+      <c r="I62" s="51"/>
       <c r="J62" s="32"/>
       <c r="K62" s="32"/>
       <c r="L62" s="39"/>
-      <c r="M62" s="32"/>
-      <c r="N62" s="32"/>
-      <c r="O62" s="32"/>
-      <c r="P62" s="32"/>
-      <c r="Q62" s="32"/>
-      <c r="R62" s="32"/>
+      <c r="M62" s="39"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="39"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="2"/>
       <c r="S62" s="32"/>
     </row>
     <row r="63" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B63" s="54"/>
       <c r="C63" s="32"/>
@@ -10628,7 +10730,7 @@
     </row>
     <row r="64" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="32"/>
@@ -10651,7 +10753,7 @@
     </row>
     <row r="65" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B65" s="54"/>
       <c r="C65" s="32"/>
@@ -10674,263 +10776,302 @@
     </row>
     <row r="66" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B66" s="54"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="32"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="52"/>
+      <c r="J66" s="32"/>
+      <c r="K66" s="32"/>
+      <c r="L66" s="39"/>
+      <c r="M66" s="32"/>
+      <c r="N66" s="32"/>
+      <c r="O66" s="32"/>
+      <c r="P66" s="32"/>
+      <c r="Q66" s="32"/>
+      <c r="R66" s="32"/>
+      <c r="S66" s="32"/>
     </row>
     <row r="67" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>62</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B67" s="54"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
+      <c r="I67" s="52"/>
+      <c r="J67" s="32"/>
+      <c r="K67" s="32"/>
+      <c r="L67" s="39"/>
+      <c r="M67" s="32"/>
+      <c r="N67" s="32"/>
+      <c r="O67" s="32"/>
+      <c r="P67" s="32"/>
+      <c r="Q67" s="32"/>
+      <c r="R67" s="32"/>
+      <c r="S67" s="32"/>
     </row>
     <row r="68" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="78" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -10942,6 +11083,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10985,39 +11133,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="71"/>
       <c r="I2" s="48"/>
@@ -11062,58 +11210,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
@@ -11138,23 +11286,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="65" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -11206,7 +11354,7 @@
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="66"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -11243,7 +11391,7 @@
       <c r="R7" s="2"/>
       <c r="S7" s="3"/>
       <c r="T7" s="66"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -11278,7 +11426,7 @@
       <c r="R8" s="2"/>
       <c r="S8" s="3"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -11313,7 +11461,7 @@
       <c r="R9" s="2"/>
       <c r="S9" s="3"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -11348,7 +11496,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="3"/>
       <c r="T10" s="66"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -11383,7 +11531,7 @@
       <c r="R11" s="2"/>
       <c r="S11" s="3"/>
       <c r="T11" s="66"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -11418,7 +11566,7 @@
       <c r="R12" s="2"/>
       <c r="S12" s="3"/>
       <c r="T12" s="66"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -11455,7 +11603,7 @@
       <c r="R13" s="2"/>
       <c r="S13" s="3"/>
       <c r="T13" s="66"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -11490,7 +11638,7 @@
       <c r="R14" s="2"/>
       <c r="S14" s="3"/>
       <c r="T14" s="66"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -11525,7 +11673,7 @@
       <c r="R15" s="2"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -11560,7 +11708,7 @@
       <c r="R16" s="2"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -13336,13 +13484,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -13354,6 +13495,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13397,41 +13545,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="95"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="48"/>
@@ -13476,58 +13624,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="86" t="s">
+      <c r="P4" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="88" t="s">
+      <c r="R4" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="65" t="s">
         <v>1</v>
       </c>
@@ -13552,23 +13700,23 @@
       <c r="I5" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="65" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="89"/>
-      <c r="R5" s="89"/>
-      <c r="S5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="90"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="90"/>
+      <c r="R5" s="90"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -13622,7 +13770,7 @@
         <v>69</v>
       </c>
       <c r="T6" s="66"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -13683,7 +13831,7 @@
         <v>69</v>
       </c>
       <c r="T7" s="66"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -13732,7 +13880,7 @@
       </c>
       <c r="S8" s="3"/>
       <c r="T8" s="66"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -13789,7 +13937,7 @@
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="66"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -13848,7 +13996,7 @@
         <v>69</v>
       </c>
       <c r="T10" s="66"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -13907,7 +14055,7 @@
         <v>69</v>
       </c>
       <c r="T11" s="66"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -13966,7 +14114,7 @@
         <v>69</v>
       </c>
       <c r="T12" s="66"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -14027,7 +14175,7 @@
         <v>69</v>
       </c>
       <c r="T13" s="66"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -14086,7 +14234,7 @@
         <v>69</v>
       </c>
       <c r="T14" s="66"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -14145,7 +14293,7 @@
         <v>69</v>
       </c>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -14200,7 +14348,7 @@
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -15952,13 +16100,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -15970,6 +16111,13 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16013,41 +16161,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-      <c r="Q1" s="92"/>
-      <c r="R1" s="92"/>
-      <c r="S1" s="92"/>
-      <c r="T1" s="92"/>
-      <c r="U1" s="92"/>
-      <c r="V1" s="92"/>
+      <c r="A1" s="84"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
       <c r="W1" s="44"/>
     </row>
     <row r="2" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95" t="s">
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="95"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="4"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -16092,58 +16240,58 @@
       <c r="W3" s="26"/>
     </row>
     <row r="4" spans="1:23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="91" t="s">
+      <c r="A4" s="88" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91" t="s">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="91" t="s">
+      <c r="K4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="91"/>
-      <c r="M4" s="88" t="s">
+      <c r="L4" s="83"/>
+      <c r="M4" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="91" t="s">
+      <c r="O4" s="83" t="s">
         <v>7</v>
       </c>
       <c r="P4" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="91" t="s">
+      <c r="Q4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="R4" s="91" t="s">
+      <c r="R4" s="83" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="90" t="s">
+      <c r="S4" s="96" t="s">
         <v>54</v>
       </c>
       <c r="T4" s="26"/>
-      <c r="U4" s="91" t="s">
+      <c r="U4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="91" t="s">
+      <c r="V4" s="83" t="s">
         <v>53</v>
       </c>
       <c r="W4" s="45"/>
     </row>
     <row r="5" spans="1:23" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="96"/>
+      <c r="A5" s="88"/>
       <c r="B5" s="41" t="s">
         <v>1</v>
       </c>
@@ -16168,23 +16316,23 @@
       <c r="I5" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="91"/>
+      <c r="J5" s="83"/>
       <c r="K5" s="41" t="s">
         <v>12</v>
       </c>
       <c r="L5" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="91"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
+      <c r="O5" s="83"/>
       <c r="P5" s="97"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="90"/>
+      <c r="Q5" s="83"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="96"/>
       <c r="T5" s="26"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
       <c r="W5" s="45"/>
     </row>
     <row r="6" spans="1:23" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -16210,7 +16358,7 @@
       <c r="R6" s="37"/>
       <c r="S6" s="3"/>
       <c r="T6" s="40"/>
-      <c r="U6" s="83" t="s">
+      <c r="U6" s="91" t="s">
         <v>18</v>
       </c>
       <c r="V6" s="3" t="s">
@@ -16241,7 +16389,7 @@
       <c r="R7" s="37"/>
       <c r="S7" s="3"/>
       <c r="T7" s="40"/>
-      <c r="U7" s="84"/>
+      <c r="U7" s="92"/>
       <c r="V7" s="3" t="s">
         <v>35</v>
       </c>
@@ -16270,7 +16418,7 @@
       <c r="R8" s="37"/>
       <c r="S8" s="3"/>
       <c r="T8" s="40"/>
-      <c r="U8" s="84"/>
+      <c r="U8" s="92"/>
       <c r="V8" s="3" t="s">
         <v>21</v>
       </c>
@@ -16299,7 +16447,7 @@
       <c r="R9" s="37"/>
       <c r="S9" s="3"/>
       <c r="T9" s="40"/>
-      <c r="U9" s="84"/>
+      <c r="U9" s="92"/>
       <c r="V9" s="3" t="s">
         <v>51</v>
       </c>
@@ -16328,7 +16476,7 @@
       <c r="R10" s="37"/>
       <c r="S10" s="3"/>
       <c r="T10" s="40"/>
-      <c r="U10" s="84"/>
+      <c r="U10" s="92"/>
       <c r="V10" s="3" t="s">
         <v>31</v>
       </c>
@@ -16357,7 +16505,7 @@
       <c r="R11" s="37"/>
       <c r="S11" s="3"/>
       <c r="T11" s="40"/>
-      <c r="U11" s="84"/>
+      <c r="U11" s="92"/>
       <c r="V11" s="3" t="s">
         <v>30</v>
       </c>
@@ -16386,7 +16534,7 @@
       <c r="R12" s="37"/>
       <c r="S12" s="3"/>
       <c r="T12" s="40"/>
-      <c r="U12" s="83" t="s">
+      <c r="U12" s="91" t="s">
         <v>19</v>
       </c>
       <c r="V12" s="3" t="s">
@@ -16417,7 +16565,7 @@
       <c r="R13" s="9"/>
       <c r="S13" s="3"/>
       <c r="T13" s="40"/>
-      <c r="U13" s="84"/>
+      <c r="U13" s="92"/>
       <c r="V13" s="3" t="s">
         <v>37</v>
       </c>
@@ -16446,7 +16594,7 @@
       <c r="R14" s="37"/>
       <c r="S14" s="3"/>
       <c r="T14" s="40"/>
-      <c r="U14" s="84"/>
+      <c r="U14" s="92"/>
       <c r="V14" s="3" t="s">
         <v>36</v>
       </c>
@@ -16475,7 +16623,7 @@
       <c r="R15" s="37"/>
       <c r="S15" s="3"/>
       <c r="T15" s="13"/>
-      <c r="U15" s="84"/>
+      <c r="U15" s="92"/>
       <c r="V15" s="3" t="s">
         <v>24</v>
       </c>
@@ -16504,7 +16652,7 @@
       <c r="R16" s="37"/>
       <c r="S16" s="3"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="85"/>
+      <c r="U16" s="93"/>
       <c r="V16" s="3" t="s">
         <v>25</v>
       </c>
@@ -17735,6 +17883,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="U6:U11"/>
+    <mergeCell ref="U12:U16"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="U4:U5"/>
     <mergeCell ref="V4:V5"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:D2"/>
@@ -17746,13 +17901,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:O5"/>
-    <mergeCell ref="U6:U11"/>
-    <mergeCell ref="U12:U16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="U4:U5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>